<commit_message>
Removed non members from points
</commit_message>
<xml_diff>
--- a/2022_summer_series_positions.xlsx
+++ b/2022_summer_series_positions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitch\Desktop\Projects\VIKA\2022_Website\website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{85F43321-837C-4896-B4F3-D4C7CE6B6CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{336BDBBE-F425-4DB7-AE6C-0A70D066E746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" activeTab="2" xr2:uid="{F04811E9-38A3-4B99-BDED-515010F258AC}"/>
+    <workbookView xWindow="16740" yWindow="1185" windowWidth="21990" windowHeight="12840" activeTab="2" xr2:uid="{F04811E9-38A3-4B99-BDED-515010F258AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Distribution" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="183">
   <si>
     <t>offset</t>
   </si>
@@ -582,6 +582,12 @@
   </si>
   <si>
     <t>Bill Karas</t>
+  </si>
+  <si>
+    <t>Hide</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -5357,14 +5363,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>600839</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>591314</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>144038</xdr:rowOff>
     </xdr:to>
@@ -5389,7 +5395,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16992600" y="571500"/>
+          <a:off x="13973175" y="571500"/>
           <a:ext cx="5477639" cy="8335538"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8675,10 +8681,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD2A9064-8326-4D83-8C00-3ADDB8778C93}">
-  <dimension ref="A1:H118"/>
+  <dimension ref="A1:I118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8693,7 +8699,7 @@
     <col min="8" max="8" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>123</v>
       </c>
@@ -8718,8 +8724,11 @@
       <c r="H1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -8736,7 +8745,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -8759,7 +8768,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>126</v>
       </c>
@@ -8779,7 +8788,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>127</v>
       </c>
@@ -8795,8 +8804,11 @@
       <c r="E5" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -8816,7 +8828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>128</v>
       </c>
@@ -8842,7 +8854,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -8868,7 +8880,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -8885,7 +8897,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>129</v>
       </c>
@@ -8902,7 +8914,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>131</v>
       </c>
@@ -8919,7 +8931,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>71</v>
       </c>
@@ -8945,7 +8957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>114</v>
       </c>
@@ -9233,7 +9245,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>56</v>
       </c>
@@ -9256,7 +9268,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>58</v>
       </c>
@@ -9270,7 +9282,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>117</v>
       </c>
@@ -9290,7 +9302,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>138</v>
       </c>
@@ -9316,7 +9328,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>139</v>
       </c>
@@ -9339,7 +9351,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -9365,7 +9377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>62</v>
       </c>
@@ -9379,7 +9391,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>120</v>
       </c>
@@ -9405,7 +9417,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>38</v>
       </c>
@@ -9422,7 +9434,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>121</v>
       </c>
@@ -9447,8 +9459,11 @@
       <c r="H42">
         <v>3</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>116</v>
       </c>
@@ -9473,8 +9488,11 @@
       <c r="H43">
         <v>7</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>140</v>
       </c>
@@ -9482,7 +9500,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>141</v>
       </c>
@@ -9508,7 +9526,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>57</v>
       </c>
@@ -9534,7 +9552,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>168</v>
       </c>
@@ -9550,8 +9568,11 @@
       <c r="E47">
         <v>10</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>169</v>
       </c>
@@ -9567,16 +9588,22 @@
       <c r="E48">
         <v>11</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>41</v>
       </c>
       <c r="B49" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>178</v>
       </c>
@@ -9587,7 +9614,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>78</v>
       </c>
@@ -9613,7 +9640,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>79</v>
       </c>
@@ -9630,7 +9657,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>143</v>
       </c>
@@ -9646,8 +9673,11 @@
       <c r="H55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>144</v>
       </c>
@@ -9673,7 +9703,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>170</v>
       </c>
@@ -9699,7 +9729,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>81</v>
       </c>
@@ -9722,7 +9752,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>43</v>
       </c>
@@ -9748,7 +9778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>3</v>
       </c>
@@ -10061,7 +10091,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>11</v>
       </c>
@@ -10087,7 +10117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>8</v>
       </c>
@@ -10110,7 +10140,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>37</v>
       </c>
@@ -10118,7 +10148,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>151</v>
       </c>
@@ -10135,7 +10165,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>12</v>
       </c>
@@ -10152,7 +10182,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>87</v>
       </c>
@@ -10169,7 +10199,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>9</v>
       </c>
@@ -10186,7 +10216,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>172</v>
       </c>
@@ -10200,7 +10230,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>59</v>
       </c>
@@ -10208,7 +10238,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>110</v>
       </c>
@@ -10233,8 +10263,11 @@
       <c r="H91">
         <v>2</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I91" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>152</v>
       </c>
@@ -10251,7 +10284,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>17</v>
       </c>
@@ -10259,7 +10292,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>84</v>
       </c>
@@ -10267,7 +10300,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>15</v>
       </c>
@@ -10293,7 +10326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>19</v>
       </c>
@@ -10319,7 +10352,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>153</v>
       </c>
@@ -10336,7 +10369,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>154</v>
       </c>
@@ -10344,7 +10377,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>155</v>
       </c>
@@ -10360,8 +10393,11 @@
       <c r="H99">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I99" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>112</v>
       </c>
@@ -10384,7 +10420,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>156</v>
       </c>
@@ -10407,7 +10443,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>21</v>
       </c>
@@ -10424,7 +10460,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>157</v>
       </c>
@@ -10432,7 +10468,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>158</v>
       </c>
@@ -10449,7 +10485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>159</v>
       </c>
@@ -10463,7 +10499,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>160</v>
       </c>
@@ -10480,7 +10516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>14</v>
       </c>
@@ -10506,7 +10542,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>173</v>
       </c>
@@ -10523,7 +10559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>16</v>
       </c>
@@ -10540,7 +10576,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>99</v>
       </c>
@@ -10554,7 +10590,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>174</v>
       </c>
@@ -10571,7 +10607,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>175</v>
       </c>
@@ -10593,8 +10629,11 @@
       <c r="H112">
         <v>8</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I112" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>176</v>
       </c>
@@ -10619,8 +10658,11 @@
       <c r="H113">
         <v>10</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I113" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>63</v>
       </c>
@@ -10637,7 +10679,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>177</v>
       </c>
@@ -10654,7 +10696,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>57</v>
       </c>
@@ -10668,7 +10710,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>179</v>
       </c>
@@ -10684,8 +10726,11 @@
       <c r="H117">
         <v>3</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I117" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>180</v>
       </c>
@@ -10710,21 +10755,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E6AF795D8A01FF43A9E4AF9E30B144DB" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0ff7acb529109b266cdfa94bf47f11ec">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a1346f0d-2271-46d3-b9c8-3d8c72d47be9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a845eecb48e3f5109706bc8393ea6c74" ns3:_="">
     <xsd:import namespace="a1346f0d-2271-46d3-b9c8-3d8c72d47be9"/>
@@ -10856,21 +10886,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8972A39A-C6AE-440C-A903-BE881E6D34A2}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FD5D83C-D53F-4CBB-B688-480C957B700B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3D20D34-01E6-4F63-B80D-EF1EFB6E6003}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10886,4 +10917,18 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FD5D83C-D53F-4CBB-B688-480C957B700B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8972A39A-C6AE-440C-A903-BE881E6D34A2}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated summer series points for race 3 and 4
</commit_message>
<xml_diff>
--- a/2022_summer_series_positions.xlsx
+++ b/2022_summer_series_positions.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitch\Desktop\Projects\VIKA\2022_Website\website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{336BDBBE-F425-4DB7-AE6C-0A70D066E746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186CD800-707B-4BA1-9F18-5BD31C03D68A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16740" yWindow="1185" windowWidth="21990" windowHeight="12840" activeTab="2" xr2:uid="{F04811E9-38A3-4B99-BDED-515010F258AC}"/>
+    <workbookView xWindow="345" yWindow="4260" windowWidth="6600" windowHeight="10305" activeTab="3" xr2:uid="{F04811E9-38A3-4B99-BDED-515010F258AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Distribution" sheetId="1" r:id="rId1"/>
     <sheet name="points_csv" sheetId="2" r:id="rId2"/>
-    <sheet name="2022_summer_series_positions" sheetId="3" r:id="rId3"/>
+    <sheet name="Race 1 2" sheetId="3" r:id="rId3"/>
+    <sheet name="Race 3 4" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">points_csv!$A$72:$F$101</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="218">
   <si>
     <t>offset</t>
   </si>
@@ -588,6 +589,111 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Race 3 - Qualifying</t>
+  </si>
+  <si>
+    <t>Race 3 - Pre-final</t>
+  </si>
+  <si>
+    <t>Race 3 - Final</t>
+  </si>
+  <si>
+    <t>Race 4 - Qualifying</t>
+  </si>
+  <si>
+    <t>Race 4 - Pre-final</t>
+  </si>
+  <si>
+    <t>Race 4 - Final</t>
+  </si>
+  <si>
+    <t>Corey Fehr</t>
+  </si>
+  <si>
+    <t>Haydn Seal-jones</t>
+  </si>
+  <si>
+    <t>Kevin Roberts</t>
+  </si>
+  <si>
+    <t>Libral Furtado</t>
+  </si>
+  <si>
+    <t>Rob Gutierrez</t>
+  </si>
+  <si>
+    <t>Jordan Wilson</t>
+  </si>
+  <si>
+    <t>Blake Wade</t>
+  </si>
+  <si>
+    <t>Anastasia Petukhova</t>
+  </si>
+  <si>
+    <t>Braydon Otto</t>
+  </si>
+  <si>
+    <t>Doug Litherland</t>
+  </si>
+  <si>
+    <t>Rod Matthews</t>
+  </si>
+  <si>
+    <t>Terry Martens</t>
+  </si>
+  <si>
+    <t>Waldo De Groot</t>
+  </si>
+  <si>
+    <t>James Bedard</t>
+  </si>
+  <si>
+    <t>William Wark</t>
+  </si>
+  <si>
+    <t>Tanner bouman</t>
+  </si>
+  <si>
+    <t>Blake Polischuk</t>
+  </si>
+  <si>
+    <t>Chris Gallaugher</t>
+  </si>
+  <si>
+    <t>cHRIS Souliotis</t>
+  </si>
+  <si>
+    <t>Mark Parry</t>
+  </si>
+  <si>
+    <t>Andrew Casey</t>
+  </si>
+  <si>
+    <t>Brett Liboiron</t>
+  </si>
+  <si>
+    <t>Brett Robinson</t>
+  </si>
+  <si>
+    <t>Ian Pirie</t>
+  </si>
+  <si>
+    <t>Joe Reaume</t>
+  </si>
+  <si>
+    <t>Matt Judge</t>
+  </si>
+  <si>
+    <t>Nolan Perry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tayler Rand </t>
+  </si>
+  <si>
+    <t>TJ Rand</t>
   </si>
 </sst>
 </file>
@@ -629,8 +735,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5395,7 +5504,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13973175" y="571500"/>
+          <a:off x="18954750" y="571500"/>
           <a:ext cx="5477639" cy="8335538"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8683,17 +8792,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD2A9064-8326-4D83-8C00-3ADDB8778C93}">
   <dimension ref="A1:I118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.140625" customWidth="1"/>
-    <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="27" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="36.7109375" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" customWidth="1"/>
     <col min="6" max="6" width="37.42578125" customWidth="1"/>
     <col min="7" max="7" width="38.140625" customWidth="1"/>
     <col min="8" max="8" width="26.140625" customWidth="1"/>
@@ -8730,154 +8839,154 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>124</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
         <v>124</v>
       </c>
       <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>167</v>
-      </c>
-      <c r="F3">
-        <v>4</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="H3">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s">
         <v>124</v>
       </c>
       <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
         <v>4</v>
       </c>
-      <c r="E4">
-        <v>1</v>
+      <c r="E4" t="s">
+        <v>167</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B5" t="s">
         <v>124</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>167</v>
-      </c>
-      <c r="I5" t="s">
-        <v>182</v>
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>127</v>
       </c>
       <c r="B6" t="s">
         <v>124</v>
       </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>3</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>167</v>
+      </c>
+      <c r="I6" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>128</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
         <v>124</v>
       </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>6</v>
-      </c>
       <c r="E7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
         <v>3</v>
       </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
       <c r="H7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>128</v>
       </c>
       <c r="B8" t="s">
         <v>124</v>
       </c>
       <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
         <v>2</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-      <c r="G8">
-        <v>2</v>
-      </c>
-      <c r="H8">
-        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -10748,9 +10857,2901 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I9">
+    <sortCondition ref="A2:A9"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ED4FDED-9BE8-4D65-815A-56099400C9CE}">
+  <dimension ref="A1:K127"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="27" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1" t="s">
+        <v>183</v>
+      </c>
+      <c r="G1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H1" t="s">
+        <v>185</v>
+      </c>
+      <c r="I1" t="s">
+        <v>186</v>
+      </c>
+      <c r="J1" t="s">
+        <v>187</v>
+      </c>
+      <c r="K1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F3">
+        <v>7</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>124</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B8" t="s">
+        <v>124</v>
+      </c>
+      <c r="G8">
+        <v>8</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>3</v>
+      </c>
+      <c r="K9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>191</v>
+      </c>
+      <c r="B10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>9</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>192</v>
+      </c>
+      <c r="B11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>6</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>6</v>
+      </c>
+      <c r="J11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>193</v>
+      </c>
+      <c r="B12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>170</v>
+      </c>
+      <c r="B15" t="s">
+        <v>130</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" t="s">
+        <v>130</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B17" t="s">
+        <v>130</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>195</v>
+      </c>
+      <c r="B18" t="s">
+        <v>130</v>
+      </c>
+      <c r="I18">
+        <v>3</v>
+      </c>
+      <c r="J18">
+        <v>3</v>
+      </c>
+      <c r="K18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" t="s">
+        <v>130</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>6</v>
+      </c>
+      <c r="E21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" t="s">
+        <v>132</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>3</v>
+      </c>
+      <c r="H22">
+        <v>3</v>
+      </c>
+      <c r="I22">
+        <v>3</v>
+      </c>
+      <c r="J22">
+        <v>2</v>
+      </c>
+      <c r="K22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <v>2</v>
+      </c>
+      <c r="J23">
+        <v>3</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>134</v>
+      </c>
+      <c r="B24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" t="s">
+        <v>132</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25">
+        <v>5</v>
+      </c>
+      <c r="G25">
+        <v>5</v>
+      </c>
+      <c r="H25">
+        <v>5</v>
+      </c>
+      <c r="I25">
+        <v>5</v>
+      </c>
+      <c r="J25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" t="s">
+        <v>132</v>
+      </c>
+      <c r="G26">
+        <v>6</v>
+      </c>
+      <c r="H26">
+        <v>6</v>
+      </c>
+      <c r="I26">
+        <v>6</v>
+      </c>
+      <c r="J26">
+        <v>5</v>
+      </c>
+      <c r="K26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" t="s">
+        <v>132</v>
+      </c>
+      <c r="C27">
+        <v>6</v>
+      </c>
+      <c r="D27">
+        <v>7</v>
+      </c>
+      <c r="E27">
+        <v>6</v>
+      </c>
+      <c r="F27">
+        <v>4</v>
+      </c>
+      <c r="G27">
+        <v>4</v>
+      </c>
+      <c r="H27">
+        <v>4</v>
+      </c>
+      <c r="I27">
+        <v>4</v>
+      </c>
+      <c r="J27">
+        <v>6</v>
+      </c>
+      <c r="K27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>196</v>
+      </c>
+      <c r="B30" t="s">
+        <v>136</v>
+      </c>
+      <c r="F30">
+        <v>17</v>
+      </c>
+      <c r="G30">
+        <v>11</v>
+      </c>
+      <c r="H30">
+        <v>10</v>
+      </c>
+      <c r="I30">
+        <v>3</v>
+      </c>
+      <c r="J30">
+        <v>13</v>
+      </c>
+      <c r="K30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" t="s">
+        <v>136</v>
+      </c>
+      <c r="F31">
+        <v>10</v>
+      </c>
+      <c r="G31">
+        <v>17</v>
+      </c>
+      <c r="H31">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>197</v>
+      </c>
+      <c r="B32" t="s">
+        <v>136</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>7</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" t="s">
+        <v>136</v>
+      </c>
+      <c r="F33">
+        <v>13</v>
+      </c>
+      <c r="G33">
+        <v>9</v>
+      </c>
+      <c r="H33">
+        <v>18</v>
+      </c>
+      <c r="I33">
+        <v>14</v>
+      </c>
+      <c r="J33">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" t="s">
+        <v>136</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
+      </c>
+      <c r="D34">
+        <v>6</v>
+      </c>
+      <c r="E34">
+        <v>13</v>
+      </c>
+      <c r="F34">
+        <v>23</v>
+      </c>
+      <c r="G34">
+        <v>22</v>
+      </c>
+      <c r="H34">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" t="s">
+        <v>136</v>
+      </c>
+      <c r="C35">
+        <v>11</v>
+      </c>
+      <c r="D35">
+        <v>11</v>
+      </c>
+      <c r="E35">
+        <v>10</v>
+      </c>
+      <c r="F35">
+        <v>3</v>
+      </c>
+      <c r="G35">
+        <v>6</v>
+      </c>
+      <c r="H35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>137</v>
+      </c>
+      <c r="B36" t="s">
+        <v>136</v>
+      </c>
+      <c r="F36">
+        <v>20</v>
+      </c>
+      <c r="G36">
+        <v>18</v>
+      </c>
+      <c r="H36">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" t="s">
+        <v>136</v>
+      </c>
+      <c r="C37">
+        <v>14</v>
+      </c>
+      <c r="D37">
+        <v>14</v>
+      </c>
+      <c r="E37">
+        <v>11</v>
+      </c>
+      <c r="F37">
+        <v>15</v>
+      </c>
+      <c r="G37">
+        <v>23</v>
+      </c>
+      <c r="H37">
+        <v>14</v>
+      </c>
+      <c r="I37">
+        <v>9</v>
+      </c>
+      <c r="J37">
+        <v>15</v>
+      </c>
+      <c r="K37">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>198</v>
+      </c>
+      <c r="B38" t="s">
+        <v>136</v>
+      </c>
+      <c r="C38">
+        <v>10</v>
+      </c>
+      <c r="D38">
+        <v>10</v>
+      </c>
+      <c r="E38">
+        <v>7</v>
+      </c>
+      <c r="F38">
+        <v>7</v>
+      </c>
+      <c r="G38">
+        <v>2</v>
+      </c>
+      <c r="H38">
+        <v>3</v>
+      </c>
+      <c r="I38">
+        <v>5</v>
+      </c>
+      <c r="J38">
+        <v>6</v>
+      </c>
+      <c r="K38">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" t="s">
+        <v>136</v>
+      </c>
+      <c r="F39">
+        <v>12</v>
+      </c>
+      <c r="G39">
+        <v>12</v>
+      </c>
+      <c r="H39">
+        <v>11</v>
+      </c>
+      <c r="I39">
+        <v>11</v>
+      </c>
+      <c r="J39">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>117</v>
+      </c>
+      <c r="B40" t="s">
+        <v>136</v>
+      </c>
+      <c r="F40">
+        <v>9</v>
+      </c>
+      <c r="G40">
+        <v>19</v>
+      </c>
+      <c r="H40">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>178</v>
+      </c>
+      <c r="B41" t="s">
+        <v>136</v>
+      </c>
+      <c r="F41">
+        <v>14</v>
+      </c>
+      <c r="G41">
+        <v>13</v>
+      </c>
+      <c r="H41">
+        <v>7</v>
+      </c>
+      <c r="I41">
+        <v>12</v>
+      </c>
+      <c r="J41">
+        <v>10</v>
+      </c>
+      <c r="K41">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>138</v>
+      </c>
+      <c r="B42" t="s">
+        <v>136</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42">
+        <v>5</v>
+      </c>
+      <c r="E42">
+        <v>6</v>
+      </c>
+      <c r="F42">
+        <v>8</v>
+      </c>
+      <c r="G42">
+        <v>3</v>
+      </c>
+      <c r="H42">
+        <v>8</v>
+      </c>
+      <c r="I42">
+        <v>15</v>
+      </c>
+      <c r="J42">
+        <v>12</v>
+      </c>
+      <c r="K42">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>139</v>
+      </c>
+      <c r="B43" t="s">
+        <v>136</v>
+      </c>
+      <c r="F43">
+        <v>21</v>
+      </c>
+      <c r="G43">
+        <v>21</v>
+      </c>
+      <c r="H43">
+        <v>19</v>
+      </c>
+      <c r="I43">
+        <v>16</v>
+      </c>
+      <c r="J43">
+        <v>16</v>
+      </c>
+      <c r="K43">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>36</v>
+      </c>
+      <c r="B44" t="s">
+        <v>136</v>
+      </c>
+      <c r="F44">
+        <v>4</v>
+      </c>
+      <c r="G44">
+        <v>4</v>
+      </c>
+      <c r="H44">
+        <v>2</v>
+      </c>
+      <c r="I44">
+        <v>6</v>
+      </c>
+      <c r="J44">
+        <v>5</v>
+      </c>
+      <c r="K44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>120</v>
+      </c>
+      <c r="B45" t="s">
+        <v>136</v>
+      </c>
+      <c r="F45">
+        <v>18</v>
+      </c>
+      <c r="G45">
+        <v>7</v>
+      </c>
+      <c r="H45">
+        <v>13</v>
+      </c>
+      <c r="I45">
+        <v>13</v>
+      </c>
+      <c r="J45">
+        <v>8</v>
+      </c>
+      <c r="K45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>38</v>
+      </c>
+      <c r="B46" t="s">
+        <v>136</v>
+      </c>
+      <c r="F46">
+        <v>19</v>
+      </c>
+      <c r="G46">
+        <v>16</v>
+      </c>
+      <c r="H46">
+        <v>17</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" t="s">
+        <v>136</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47">
+        <v>4</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="G47">
+        <v>15</v>
+      </c>
+      <c r="H47">
+        <v>6</v>
+      </c>
+      <c r="J47">
+        <v>2</v>
+      </c>
+      <c r="K47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>121</v>
+      </c>
+      <c r="B48" t="s">
+        <v>136</v>
+      </c>
+      <c r="C48">
+        <v>6</v>
+      </c>
+      <c r="D48">
+        <v>8</v>
+      </c>
+      <c r="E48">
+        <v>8</v>
+      </c>
+      <c r="F48">
+        <v>5</v>
+      </c>
+      <c r="G48">
+        <v>14</v>
+      </c>
+      <c r="H48">
+        <v>15</v>
+      </c>
+      <c r="I48">
+        <v>2</v>
+      </c>
+      <c r="J48">
+        <v>4</v>
+      </c>
+      <c r="K48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>199</v>
+      </c>
+      <c r="B49" t="s">
+        <v>136</v>
+      </c>
+      <c r="C49">
+        <v>12</v>
+      </c>
+      <c r="D49">
+        <v>13</v>
+      </c>
+      <c r="F49">
+        <v>6</v>
+      </c>
+      <c r="G49">
+        <v>5</v>
+      </c>
+      <c r="H49">
+        <v>5</v>
+      </c>
+      <c r="I49">
+        <v>4</v>
+      </c>
+      <c r="J49">
+        <v>3</v>
+      </c>
+      <c r="K49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>116</v>
+      </c>
+      <c r="B50" t="s">
+        <v>136</v>
+      </c>
+      <c r="C50">
+        <v>8</v>
+      </c>
+      <c r="D50">
+        <v>7</v>
+      </c>
+      <c r="E50">
+        <v>4</v>
+      </c>
+      <c r="F50">
+        <v>16</v>
+      </c>
+      <c r="G50">
+        <v>8</v>
+      </c>
+      <c r="H50">
+        <v>9</v>
+      </c>
+      <c r="I50">
+        <v>8</v>
+      </c>
+      <c r="J50">
+        <v>14</v>
+      </c>
+      <c r="K50">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>200</v>
+      </c>
+      <c r="B51" t="s">
+        <v>136</v>
+      </c>
+      <c r="C51">
+        <v>15</v>
+      </c>
+      <c r="D51">
+        <v>16</v>
+      </c>
+      <c r="F51">
+        <v>22</v>
+      </c>
+      <c r="G51">
+        <v>20</v>
+      </c>
+      <c r="H51">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>201</v>
+      </c>
+      <c r="B52" t="s">
+        <v>136</v>
+      </c>
+      <c r="C52">
+        <v>9</v>
+      </c>
+      <c r="D52">
+        <v>12</v>
+      </c>
+      <c r="E52">
+        <v>9</v>
+      </c>
+      <c r="F52">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>141</v>
+      </c>
+      <c r="B53" t="s">
+        <v>136</v>
+      </c>
+      <c r="C53">
+        <v>7</v>
+      </c>
+      <c r="D53">
+        <v>3</v>
+      </c>
+      <c r="E53">
+        <v>5</v>
+      </c>
+      <c r="F53">
+        <v>11</v>
+      </c>
+      <c r="G53">
+        <v>10</v>
+      </c>
+      <c r="H53">
+        <v>22</v>
+      </c>
+      <c r="I53">
+        <v>10</v>
+      </c>
+      <c r="J53">
+        <v>7</v>
+      </c>
+      <c r="K53">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>170</v>
+      </c>
+      <c r="B56" t="s">
+        <v>142</v>
+      </c>
+      <c r="F56">
+        <v>3</v>
+      </c>
+      <c r="G56">
+        <v>3</v>
+      </c>
+      <c r="H56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>78</v>
+      </c>
+      <c r="B57" t="s">
+        <v>142</v>
+      </c>
+      <c r="C57">
+        <v>4</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57">
+        <v>3</v>
+      </c>
+      <c r="F57">
+        <v>4</v>
+      </c>
+      <c r="G57">
+        <v>2</v>
+      </c>
+      <c r="H57">
+        <v>3</v>
+      </c>
+      <c r="I57">
+        <v>3</v>
+      </c>
+      <c r="J57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>202</v>
+      </c>
+      <c r="B58" t="s">
+        <v>142</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="I58">
+        <v>1</v>
+      </c>
+      <c r="J58">
+        <v>1</v>
+      </c>
+      <c r="K58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>144</v>
+      </c>
+      <c r="B59" t="s">
+        <v>142</v>
+      </c>
+      <c r="C59">
+        <v>3</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>2</v>
+      </c>
+      <c r="F59">
+        <v>2</v>
+      </c>
+      <c r="G59">
+        <v>5</v>
+      </c>
+      <c r="H59">
+        <v>2</v>
+      </c>
+      <c r="I59">
+        <v>2</v>
+      </c>
+      <c r="J59">
+        <v>2</v>
+      </c>
+      <c r="K59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>203</v>
+      </c>
+      <c r="B60" t="s">
+        <v>142</v>
+      </c>
+      <c r="F60">
+        <v>5</v>
+      </c>
+      <c r="G60">
+        <v>4</v>
+      </c>
+      <c r="H60">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>4</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>81</v>
+      </c>
+      <c r="B63" t="s">
+        <v>80</v>
+      </c>
+      <c r="G63">
+        <v>2</v>
+      </c>
+      <c r="H63">
+        <v>2</v>
+      </c>
+      <c r="I63">
+        <v>2</v>
+      </c>
+      <c r="J63">
+        <v>2</v>
+      </c>
+      <c r="K63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>204</v>
+      </c>
+      <c r="B64" t="s">
+        <v>80</v>
+      </c>
+      <c r="C64">
+        <v>2</v>
+      </c>
+      <c r="D64">
+        <v>3</v>
+      </c>
+      <c r="E64" t="s">
+        <v>167</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+      <c r="G64">
+        <v>1</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64">
+        <v>1</v>
+      </c>
+      <c r="J64">
+        <v>1</v>
+      </c>
+      <c r="K64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C66">
+        <v>2</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>3</v>
+      </c>
+      <c r="B67" t="s">
+        <v>145</v>
+      </c>
+      <c r="C67">
+        <v>6</v>
+      </c>
+      <c r="D67">
+        <v>14</v>
+      </c>
+      <c r="F67">
+        <v>7</v>
+      </c>
+      <c r="G67">
+        <v>7</v>
+      </c>
+      <c r="H67">
+        <v>13</v>
+      </c>
+      <c r="I67">
+        <v>5</v>
+      </c>
+      <c r="J67">
+        <v>5</v>
+      </c>
+      <c r="K67">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>2</v>
+      </c>
+      <c r="B68" t="s">
+        <v>145</v>
+      </c>
+      <c r="C68">
+        <v>14</v>
+      </c>
+      <c r="D68">
+        <v>17</v>
+      </c>
+      <c r="E68">
+        <v>15</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+      <c r="I68">
+        <v>1</v>
+      </c>
+      <c r="J68">
+        <v>19</v>
+      </c>
+      <c r="K68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>146</v>
+      </c>
+      <c r="B69" t="s">
+        <v>145</v>
+      </c>
+      <c r="C69">
+        <v>3</v>
+      </c>
+      <c r="D69">
+        <v>2</v>
+      </c>
+      <c r="E69">
+        <v>4</v>
+      </c>
+      <c r="F69">
+        <v>20</v>
+      </c>
+      <c r="I69">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>205</v>
+      </c>
+      <c r="B70" t="s">
+        <v>145</v>
+      </c>
+      <c r="C70">
+        <v>7</v>
+      </c>
+      <c r="D70">
+        <v>5</v>
+      </c>
+      <c r="E70">
+        <v>17</v>
+      </c>
+      <c r="F70">
+        <v>17</v>
+      </c>
+      <c r="G70">
+        <v>17</v>
+      </c>
+      <c r="H70">
+        <v>17</v>
+      </c>
+      <c r="I70">
+        <v>14</v>
+      </c>
+      <c r="J70">
+        <v>12</v>
+      </c>
+      <c r="K70">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>105</v>
+      </c>
+      <c r="B71" t="s">
+        <v>145</v>
+      </c>
+      <c r="F71">
+        <v>16</v>
+      </c>
+      <c r="G71">
+        <v>18</v>
+      </c>
+      <c r="I71">
+        <v>12</v>
+      </c>
+      <c r="J71">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>84</v>
+      </c>
+      <c r="B72" t="s">
+        <v>145</v>
+      </c>
+      <c r="F72">
+        <v>5</v>
+      </c>
+      <c r="G72">
+        <v>5</v>
+      </c>
+      <c r="H72">
+        <v>4</v>
+      </c>
+      <c r="I72">
+        <v>6</v>
+      </c>
+      <c r="J72">
+        <v>2</v>
+      </c>
+      <c r="K72">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>206</v>
+      </c>
+      <c r="B73" t="s">
+        <v>145</v>
+      </c>
+      <c r="C73">
+        <v>2</v>
+      </c>
+      <c r="D73">
+        <v>15</v>
+      </c>
+      <c r="E73">
+        <v>3</v>
+      </c>
+      <c r="I73">
+        <v>16</v>
+      </c>
+      <c r="J73">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>207</v>
+      </c>
+      <c r="B74" t="s">
+        <v>145</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="G74">
+        <v>16</v>
+      </c>
+      <c r="H74">
+        <v>16</v>
+      </c>
+      <c r="I74">
+        <v>13</v>
+      </c>
+      <c r="J74">
+        <v>11</v>
+      </c>
+      <c r="K74">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>4</v>
+      </c>
+      <c r="B75" t="s">
+        <v>145</v>
+      </c>
+      <c r="C75">
+        <v>9</v>
+      </c>
+      <c r="D75">
+        <v>7</v>
+      </c>
+      <c r="E75">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>106</v>
+      </c>
+      <c r="B76" t="s">
+        <v>145</v>
+      </c>
+      <c r="D76">
+        <v>8</v>
+      </c>
+      <c r="E76">
+        <v>8</v>
+      </c>
+      <c r="F76">
+        <v>15</v>
+      </c>
+      <c r="G76">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>6</v>
+      </c>
+      <c r="B77" t="s">
+        <v>145</v>
+      </c>
+      <c r="D77">
+        <v>16</v>
+      </c>
+      <c r="E77">
+        <v>16</v>
+      </c>
+      <c r="F77">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>86</v>
+      </c>
+      <c r="B78" t="s">
+        <v>145</v>
+      </c>
+      <c r="C78">
+        <v>4</v>
+      </c>
+      <c r="D78">
+        <v>4</v>
+      </c>
+      <c r="E78">
+        <v>5</v>
+      </c>
+      <c r="H78">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>147</v>
+      </c>
+      <c r="B79" t="s">
+        <v>145</v>
+      </c>
+      <c r="F79">
+        <v>18</v>
+      </c>
+      <c r="G79">
+        <v>15</v>
+      </c>
+      <c r="H79">
+        <v>15</v>
+      </c>
+      <c r="I79">
+        <v>15</v>
+      </c>
+      <c r="J79">
+        <v>13</v>
+      </c>
+      <c r="K79">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>98</v>
+      </c>
+      <c r="B80" t="s">
+        <v>145</v>
+      </c>
+      <c r="F80">
+        <v>13</v>
+      </c>
+      <c r="G80">
+        <v>13</v>
+      </c>
+      <c r="H80">
+        <v>11</v>
+      </c>
+      <c r="I80">
+        <v>9</v>
+      </c>
+      <c r="J80">
+        <v>8</v>
+      </c>
+      <c r="K80">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>148</v>
+      </c>
+      <c r="B81" t="s">
+        <v>145</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+      <c r="D81">
+        <v>2</v>
+      </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
+      <c r="F81">
+        <v>10</v>
+      </c>
+      <c r="G81">
+        <v>11</v>
+      </c>
+      <c r="H81">
+        <v>10</v>
+      </c>
+      <c r="J81">
+        <v>10</v>
+      </c>
+      <c r="K81">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>88</v>
+      </c>
+      <c r="B82" t="s">
+        <v>145</v>
+      </c>
+      <c r="F82">
+        <v>3</v>
+      </c>
+      <c r="G82">
+        <v>4</v>
+      </c>
+      <c r="H82">
+        <v>6</v>
+      </c>
+      <c r="I82">
+        <v>4</v>
+      </c>
+      <c r="J82">
+        <v>4</v>
+      </c>
+      <c r="K82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>12</v>
+      </c>
+      <c r="B83" t="s">
+        <v>145</v>
+      </c>
+      <c r="F83">
+        <v>2</v>
+      </c>
+      <c r="G83">
+        <v>2</v>
+      </c>
+      <c r="H83">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>154</v>
+      </c>
+      <c r="B84" t="s">
+        <v>145</v>
+      </c>
+      <c r="J84">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>104</v>
+      </c>
+      <c r="B85" t="s">
+        <v>145</v>
+      </c>
+      <c r="F85">
+        <v>19</v>
+      </c>
+      <c r="G85">
+        <v>12</v>
+      </c>
+      <c r="H85">
+        <v>18</v>
+      </c>
+      <c r="I85">
+        <v>18</v>
+      </c>
+      <c r="J85">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>208</v>
+      </c>
+      <c r="B86" t="s">
+        <v>145</v>
+      </c>
+      <c r="F86">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>150</v>
+      </c>
+      <c r="B87" t="s">
+        <v>145</v>
+      </c>
+      <c r="C87">
+        <v>13</v>
+      </c>
+      <c r="D87">
+        <v>13</v>
+      </c>
+      <c r="E87">
+        <v>13</v>
+      </c>
+      <c r="F87">
+        <v>9</v>
+      </c>
+      <c r="G87">
+        <v>9</v>
+      </c>
+      <c r="H87">
+        <v>8</v>
+      </c>
+      <c r="I87">
+        <v>7</v>
+      </c>
+      <c r="J87">
+        <v>6</v>
+      </c>
+      <c r="K87">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>34</v>
+      </c>
+      <c r="B88" t="s">
+        <v>145</v>
+      </c>
+      <c r="C88">
+        <v>10</v>
+      </c>
+      <c r="D88">
+        <v>12</v>
+      </c>
+      <c r="E88">
+        <v>6</v>
+      </c>
+      <c r="F88">
+        <v>6</v>
+      </c>
+      <c r="G88">
+        <v>6</v>
+      </c>
+      <c r="H88">
+        <v>5</v>
+      </c>
+      <c r="I88">
+        <v>2</v>
+      </c>
+      <c r="J88">
+        <v>3</v>
+      </c>
+      <c r="K88">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>11</v>
+      </c>
+      <c r="B89" t="s">
+        <v>145</v>
+      </c>
+      <c r="F89">
+        <v>4</v>
+      </c>
+      <c r="G89">
+        <v>3</v>
+      </c>
+      <c r="H89">
+        <v>2</v>
+      </c>
+      <c r="I89">
+        <v>3</v>
+      </c>
+      <c r="J89">
+        <v>1</v>
+      </c>
+      <c r="K89">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>8</v>
+      </c>
+      <c r="B90" t="s">
+        <v>145</v>
+      </c>
+      <c r="C90">
+        <v>12</v>
+      </c>
+      <c r="D90">
+        <v>10</v>
+      </c>
+      <c r="E90">
+        <v>11</v>
+      </c>
+      <c r="F90">
+        <v>11</v>
+      </c>
+      <c r="G90">
+        <v>10</v>
+      </c>
+      <c r="H90">
+        <v>9</v>
+      </c>
+      <c r="I90">
+        <v>10</v>
+      </c>
+      <c r="J90">
+        <v>9</v>
+      </c>
+      <c r="K90">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>37</v>
+      </c>
+      <c r="B91" t="s">
+        <v>145</v>
+      </c>
+      <c r="F91">
+        <v>14</v>
+      </c>
+      <c r="G91">
+        <v>14</v>
+      </c>
+      <c r="H91">
+        <v>14</v>
+      </c>
+      <c r="I91">
+        <v>11</v>
+      </c>
+      <c r="J91">
+        <v>16</v>
+      </c>
+      <c r="K91">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>151</v>
+      </c>
+      <c r="B92" t="s">
+        <v>145</v>
+      </c>
+      <c r="C92">
+        <v>5</v>
+      </c>
+      <c r="D92">
+        <v>3</v>
+      </c>
+      <c r="E92">
+        <v>2</v>
+      </c>
+      <c r="F92">
+        <v>8</v>
+      </c>
+      <c r="G92">
+        <v>8</v>
+      </c>
+      <c r="H92">
+        <v>7</v>
+      </c>
+      <c r="I92">
+        <v>8</v>
+      </c>
+      <c r="J92">
+        <v>7</v>
+      </c>
+      <c r="K92">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C93">
+        <v>8</v>
+      </c>
+      <c r="D93">
+        <v>6</v>
+      </c>
+      <c r="E93">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C94">
+        <v>11</v>
+      </c>
+      <c r="D94">
+        <v>9</v>
+      </c>
+      <c r="E94">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>59</v>
+      </c>
+      <c r="B95" t="s">
+        <v>10</v>
+      </c>
+      <c r="I95">
+        <v>15</v>
+      </c>
+      <c r="K95">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>209</v>
+      </c>
+      <c r="B96" t="s">
+        <v>10</v>
+      </c>
+      <c r="F96">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>99</v>
+      </c>
+      <c r="B97" t="s">
+        <v>10</v>
+      </c>
+      <c r="C97">
+        <v>3</v>
+      </c>
+      <c r="D97">
+        <v>16</v>
+      </c>
+      <c r="E97">
+        <v>3</v>
+      </c>
+      <c r="F97">
+        <v>17</v>
+      </c>
+      <c r="G97">
+        <v>13</v>
+      </c>
+      <c r="H97">
+        <v>10</v>
+      </c>
+      <c r="I97">
+        <v>10</v>
+      </c>
+      <c r="J97">
+        <v>9</v>
+      </c>
+      <c r="K97">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>210</v>
+      </c>
+      <c r="B98" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>211</v>
+      </c>
+      <c r="B99" t="s">
+        <v>10</v>
+      </c>
+      <c r="C99">
+        <v>12</v>
+      </c>
+      <c r="D99">
+        <v>12</v>
+      </c>
+      <c r="E99">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>17</v>
+      </c>
+      <c r="B100" t="s">
+        <v>10</v>
+      </c>
+      <c r="C100">
+        <v>7</v>
+      </c>
+      <c r="D100">
+        <v>7</v>
+      </c>
+      <c r="E100">
+        <v>12</v>
+      </c>
+      <c r="F100">
+        <v>14</v>
+      </c>
+      <c r="G100">
+        <v>19</v>
+      </c>
+      <c r="H100">
+        <v>14</v>
+      </c>
+      <c r="I100">
+        <v>14</v>
+      </c>
+      <c r="J100">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>15</v>
+      </c>
+      <c r="B101" t="s">
+        <v>10</v>
+      </c>
+      <c r="C101">
+        <v>9</v>
+      </c>
+      <c r="E101">
+        <v>6</v>
+      </c>
+      <c r="F101">
+        <v>16</v>
+      </c>
+      <c r="G101">
+        <v>14</v>
+      </c>
+      <c r="H101">
+        <v>13</v>
+      </c>
+      <c r="I101">
+        <v>13</v>
+      </c>
+      <c r="J101">
+        <v>14</v>
+      </c>
+      <c r="K101">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>19</v>
+      </c>
+      <c r="B102" t="s">
+        <v>10</v>
+      </c>
+      <c r="C102">
+        <v>10</v>
+      </c>
+      <c r="D102">
+        <v>6</v>
+      </c>
+      <c r="E102">
+        <v>5</v>
+      </c>
+      <c r="F102">
+        <v>6</v>
+      </c>
+      <c r="G102">
+        <v>2</v>
+      </c>
+      <c r="H102">
+        <v>3</v>
+      </c>
+      <c r="I102">
+        <v>6</v>
+      </c>
+      <c r="K102">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B103" t="s">
+        <v>10</v>
+      </c>
+      <c r="C103">
+        <v>2</v>
+      </c>
+      <c r="D103">
+        <v>2</v>
+      </c>
+      <c r="E103">
+        <v>2</v>
+      </c>
+      <c r="F103">
+        <v>19</v>
+      </c>
+      <c r="G103">
+        <v>15</v>
+      </c>
+      <c r="H103">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>212</v>
+      </c>
+      <c r="B104" t="s">
+        <v>10</v>
+      </c>
+      <c r="C104">
+        <v>5</v>
+      </c>
+      <c r="D104">
+        <v>3</v>
+      </c>
+      <c r="E104">
+        <v>15</v>
+      </c>
+      <c r="F104">
+        <v>2</v>
+      </c>
+      <c r="G104">
+        <v>4</v>
+      </c>
+      <c r="H104">
+        <v>2</v>
+      </c>
+      <c r="I104">
+        <v>2</v>
+      </c>
+      <c r="J104">
+        <v>3</v>
+      </c>
+      <c r="K104">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>175</v>
+      </c>
+      <c r="B105" t="s">
+        <v>10</v>
+      </c>
+      <c r="F105">
+        <v>13</v>
+      </c>
+      <c r="G105">
+        <v>17</v>
+      </c>
+      <c r="H105">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>213</v>
+      </c>
+      <c r="B106" t="s">
+        <v>10</v>
+      </c>
+      <c r="C106">
+        <v>11</v>
+      </c>
+      <c r="E106">
+        <v>10</v>
+      </c>
+      <c r="I106">
+        <v>12</v>
+      </c>
+      <c r="J106">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>155</v>
+      </c>
+      <c r="B107" t="s">
+        <v>10</v>
+      </c>
+      <c r="C107">
+        <v>8</v>
+      </c>
+      <c r="D107">
+        <v>9</v>
+      </c>
+      <c r="E107">
+        <v>8</v>
+      </c>
+      <c r="F107">
+        <v>1</v>
+      </c>
+      <c r="G107">
+        <v>1</v>
+      </c>
+      <c r="H107">
+        <v>1</v>
+      </c>
+      <c r="I107">
+        <v>1</v>
+      </c>
+      <c r="J107">
+        <v>1</v>
+      </c>
+      <c r="K107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>214</v>
+      </c>
+      <c r="B108" t="s">
+        <v>10</v>
+      </c>
+      <c r="F108">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>112</v>
+      </c>
+      <c r="B109" t="s">
+        <v>10</v>
+      </c>
+      <c r="C109">
+        <v>4</v>
+      </c>
+      <c r="D109">
+        <v>4</v>
+      </c>
+      <c r="E109">
+        <v>7</v>
+      </c>
+      <c r="G109">
+        <v>12</v>
+      </c>
+      <c r="H109">
+        <v>8</v>
+      </c>
+      <c r="I109">
+        <v>5</v>
+      </c>
+      <c r="J109">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>156</v>
+      </c>
+      <c r="B110" t="s">
+        <v>10</v>
+      </c>
+      <c r="F110">
+        <v>3</v>
+      </c>
+      <c r="G110">
+        <v>5</v>
+      </c>
+      <c r="H110">
+        <v>11</v>
+      </c>
+      <c r="I110">
+        <v>9</v>
+      </c>
+      <c r="J110">
+        <v>8</v>
+      </c>
+      <c r="K110">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>174</v>
+      </c>
+      <c r="B111" t="s">
+        <v>10</v>
+      </c>
+      <c r="F111">
+        <v>18</v>
+      </c>
+      <c r="G111">
+        <v>16</v>
+      </c>
+      <c r="H111">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>21</v>
+      </c>
+      <c r="B112" t="s">
+        <v>10</v>
+      </c>
+      <c r="F112">
+        <v>10</v>
+      </c>
+      <c r="G112">
+        <v>10</v>
+      </c>
+      <c r="H112">
+        <v>7</v>
+      </c>
+      <c r="I112">
+        <v>11</v>
+      </c>
+      <c r="J112">
+        <v>4</v>
+      </c>
+      <c r="K112">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>215</v>
+      </c>
+      <c r="B113" t="s">
+        <v>10</v>
+      </c>
+      <c r="F113">
+        <v>15</v>
+      </c>
+      <c r="G113">
+        <v>18</v>
+      </c>
+      <c r="H113">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>33</v>
+      </c>
+      <c r="B114" t="s">
+        <v>10</v>
+      </c>
+      <c r="D114">
+        <v>11</v>
+      </c>
+      <c r="E114">
+        <v>7</v>
+      </c>
+      <c r="F114">
+        <v>8</v>
+      </c>
+      <c r="G114">
+        <v>6</v>
+      </c>
+      <c r="H114">
+        <v>4</v>
+      </c>
+      <c r="I114">
+        <v>3</v>
+      </c>
+      <c r="J114">
+        <v>6</v>
+      </c>
+      <c r="K114">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>97</v>
+      </c>
+      <c r="B115" t="s">
+        <v>10</v>
+      </c>
+      <c r="C115">
+        <v>15</v>
+      </c>
+      <c r="D115">
+        <v>10</v>
+      </c>
+      <c r="F115">
+        <v>9</v>
+      </c>
+      <c r="G115">
+        <v>9</v>
+      </c>
+      <c r="H115">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>158</v>
+      </c>
+      <c r="B116" t="s">
+        <v>10</v>
+      </c>
+      <c r="C116">
+        <v>1</v>
+      </c>
+      <c r="D116">
+        <v>1</v>
+      </c>
+      <c r="E116">
+        <v>1</v>
+      </c>
+      <c r="F116">
+        <v>4</v>
+      </c>
+      <c r="G116">
+        <v>3</v>
+      </c>
+      <c r="H116">
+        <v>5</v>
+      </c>
+      <c r="I116">
+        <v>4</v>
+      </c>
+      <c r="J116">
+        <v>2</v>
+      </c>
+      <c r="K116">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>159</v>
+      </c>
+      <c r="B117" t="s">
+        <v>10</v>
+      </c>
+      <c r="F117">
+        <v>7</v>
+      </c>
+      <c r="G117">
+        <v>11</v>
+      </c>
+      <c r="H117">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>216</v>
+      </c>
+      <c r="B118" t="s">
+        <v>10</v>
+      </c>
+      <c r="C118">
+        <v>6</v>
+      </c>
+      <c r="D118">
+        <v>8</v>
+      </c>
+      <c r="E118">
+        <v>9</v>
+      </c>
+      <c r="J118">
+        <v>11</v>
+      </c>
+      <c r="K118">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>176</v>
+      </c>
+      <c r="B119" t="s">
+        <v>10</v>
+      </c>
+      <c r="F119">
+        <v>20</v>
+      </c>
+      <c r="I119">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>217</v>
+      </c>
+      <c r="B120" t="s">
+        <v>10</v>
+      </c>
+      <c r="F120">
+        <v>12</v>
+      </c>
+      <c r="G120">
+        <v>8</v>
+      </c>
+      <c r="H120">
+        <v>6</v>
+      </c>
+      <c r="I120">
+        <v>8</v>
+      </c>
+      <c r="J120">
+        <v>5</v>
+      </c>
+      <c r="K120">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>63</v>
+      </c>
+      <c r="B121" t="s">
+        <v>10</v>
+      </c>
+      <c r="F121">
+        <v>22</v>
+      </c>
+      <c r="I121">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>14</v>
+      </c>
+      <c r="B122" t="s">
+        <v>10</v>
+      </c>
+      <c r="F122">
+        <v>5</v>
+      </c>
+      <c r="G122">
+        <v>7</v>
+      </c>
+      <c r="H122">
+        <v>9</v>
+      </c>
+      <c r="I122">
+        <v>7</v>
+      </c>
+      <c r="J122">
+        <v>7</v>
+      </c>
+      <c r="K122">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C123">
+        <v>14</v>
+      </c>
+      <c r="D123">
+        <v>13</v>
+      </c>
+      <c r="E123">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C124">
+        <v>16</v>
+      </c>
+      <c r="D124">
+        <v>14</v>
+      </c>
+      <c r="E124">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C125">
+        <v>17</v>
+      </c>
+      <c r="D125">
+        <v>15</v>
+      </c>
+      <c r="E125">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C126">
+        <v>18</v>
+      </c>
+      <c r="D126">
+        <v>11</v>
+      </c>
+      <c r="E126">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D127">
+        <v>5</v>
+      </c>
+      <c r="E127">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -10887,18 +13888,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10920,15 +13921,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8972A39A-C6AE-440C-A903-BE881E6D34A2}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FD5D83C-D53F-4CBB-B688-480C957B700B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8972A39A-C6AE-440C-A903-BE881E6D34A2}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
 </file>
</xml_diff>